<commit_message>
Multiple changes after first corrections from KMT Staff
</commit_message>
<xml_diff>
--- a/Results-ExportTemplate.xlsx
+++ b/Results-ExportTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28913"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Darshan\Downloads\KMTL_Working\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Darshan\Desktop\BMGValuesCheckingTool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8832418A-5DC6-45FB-ADCC-412181CA69F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD0134F4-E3AE-4753-9ABF-1655981B9143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,102 +36,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>MATERIAL ID</t>
+    <t>Dimensional Values</t>
   </si>
   <si>
-    <t>Condition</t>
+    <t>Catalogue ID</t>
   </si>
   <si>
-    <t>M1</t>
-  </si>
-  <si>
-    <t>M2</t>
-  </si>
-  <si>
-    <t>M3</t>
-  </si>
-  <si>
-    <t>M4</t>
-  </si>
-  <si>
-    <t>M5</t>
-  </si>
-  <si>
-    <t>M6</t>
-  </si>
-  <si>
-    <t>M7</t>
-  </si>
-  <si>
-    <t>M8</t>
-  </si>
-  <si>
-    <t>M9</t>
-  </si>
-  <si>
-    <t>M10</t>
-  </si>
-  <si>
-    <t>M11</t>
-  </si>
-  <si>
-    <t>M12</t>
-  </si>
-  <si>
-    <t>M13</t>
-  </si>
-  <si>
-    <t>M14</t>
-  </si>
-  <si>
-    <t>M15</t>
-  </si>
-  <si>
-    <t>M16</t>
-  </si>
-  <si>
-    <t>M17</t>
-  </si>
-  <si>
-    <t>M18</t>
-  </si>
-  <si>
-    <t>M19</t>
-  </si>
-  <si>
-    <t>M20</t>
-  </si>
-  <si>
-    <t>M21</t>
-  </si>
-  <si>
-    <t>M22</t>
-  </si>
-  <si>
-    <t>M23</t>
-  </si>
-  <si>
-    <t>M24</t>
-  </si>
-  <si>
-    <t>M25</t>
-  </si>
-  <si>
-    <t>M26</t>
-  </si>
-  <si>
-    <t>M27</t>
-  </si>
-  <si>
-    <t>M28</t>
-  </si>
-  <si>
-    <t>M29</t>
-  </si>
-  <si>
-    <t>M30</t>
+    <t>RESULT</t>
   </si>
 </sst>
 </file>
@@ -179,7 +92,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -202,11 +115,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -222,6 +172,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -586,101 +545,43 @@
   <sheetData>
     <row r="1" spans="1:32" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="8"/>
+      <c r="AA1" s="8"/>
+      <c r="AB1" s="8"/>
+      <c r="AC1" s="8"/>
+      <c r="AD1" s="8"/>
+      <c r="AE1" s="8"/>
+      <c r="AF1" s="9"/>
     </row>
     <row r="2" spans="1:32" ht="39.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A2" s="5"/>
@@ -7768,7 +7669,198 @@
       <c r="AF201" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="200">
+  <mergeCells count="201">
+    <mergeCell ref="C1:AF1"/>
+    <mergeCell ref="A192:A193"/>
+    <mergeCell ref="B192:B193"/>
+    <mergeCell ref="A194:A195"/>
+    <mergeCell ref="B194:B195"/>
+    <mergeCell ref="A196:A197"/>
+    <mergeCell ref="B196:B197"/>
+    <mergeCell ref="A198:A199"/>
+    <mergeCell ref="B198:B199"/>
+    <mergeCell ref="A200:A201"/>
+    <mergeCell ref="B200:B201"/>
+    <mergeCell ref="A182:A183"/>
+    <mergeCell ref="B182:B183"/>
+    <mergeCell ref="A184:A185"/>
+    <mergeCell ref="B184:B185"/>
+    <mergeCell ref="A186:A187"/>
+    <mergeCell ref="B186:B187"/>
+    <mergeCell ref="A188:A189"/>
+    <mergeCell ref="B188:B189"/>
+    <mergeCell ref="A190:A191"/>
+    <mergeCell ref="B190:B191"/>
+    <mergeCell ref="A172:A173"/>
+    <mergeCell ref="B172:B173"/>
+    <mergeCell ref="A174:A175"/>
+    <mergeCell ref="B174:B175"/>
+    <mergeCell ref="A176:A177"/>
+    <mergeCell ref="B176:B177"/>
+    <mergeCell ref="A178:A179"/>
+    <mergeCell ref="B178:B179"/>
+    <mergeCell ref="A180:A181"/>
+    <mergeCell ref="B180:B181"/>
+    <mergeCell ref="A162:A163"/>
+    <mergeCell ref="B162:B163"/>
+    <mergeCell ref="A164:A165"/>
+    <mergeCell ref="B164:B165"/>
+    <mergeCell ref="A166:A167"/>
+    <mergeCell ref="B166:B167"/>
+    <mergeCell ref="A168:A169"/>
+    <mergeCell ref="B168:B169"/>
+    <mergeCell ref="A170:A171"/>
+    <mergeCell ref="B170:B171"/>
+    <mergeCell ref="A152:A153"/>
+    <mergeCell ref="B152:B153"/>
+    <mergeCell ref="A154:A155"/>
+    <mergeCell ref="B154:B155"/>
+    <mergeCell ref="A156:A157"/>
+    <mergeCell ref="B156:B157"/>
+    <mergeCell ref="A158:A159"/>
+    <mergeCell ref="B158:B159"/>
+    <mergeCell ref="A160:A161"/>
+    <mergeCell ref="B160:B161"/>
+    <mergeCell ref="A142:A143"/>
+    <mergeCell ref="B142:B143"/>
+    <mergeCell ref="A144:A145"/>
+    <mergeCell ref="B144:B145"/>
+    <mergeCell ref="A146:A147"/>
+    <mergeCell ref="B146:B147"/>
+    <mergeCell ref="A148:A149"/>
+    <mergeCell ref="B148:B149"/>
+    <mergeCell ref="A150:A151"/>
+    <mergeCell ref="B150:B151"/>
+    <mergeCell ref="A132:A133"/>
+    <mergeCell ref="B132:B133"/>
+    <mergeCell ref="A134:A135"/>
+    <mergeCell ref="B134:B135"/>
+    <mergeCell ref="A136:A137"/>
+    <mergeCell ref="B136:B137"/>
+    <mergeCell ref="A138:A139"/>
+    <mergeCell ref="B138:B139"/>
+    <mergeCell ref="A140:A141"/>
+    <mergeCell ref="B140:B141"/>
+    <mergeCell ref="A122:A123"/>
+    <mergeCell ref="B122:B123"/>
+    <mergeCell ref="A124:A125"/>
+    <mergeCell ref="B124:B125"/>
+    <mergeCell ref="A126:A127"/>
+    <mergeCell ref="B126:B127"/>
+    <mergeCell ref="A128:A129"/>
+    <mergeCell ref="B128:B129"/>
+    <mergeCell ref="A130:A131"/>
+    <mergeCell ref="B130:B131"/>
+    <mergeCell ref="A112:A113"/>
+    <mergeCell ref="B112:B113"/>
+    <mergeCell ref="A114:A115"/>
+    <mergeCell ref="B114:B115"/>
+    <mergeCell ref="A116:A117"/>
+    <mergeCell ref="B116:B117"/>
+    <mergeCell ref="A118:A119"/>
+    <mergeCell ref="B118:B119"/>
+    <mergeCell ref="A120:A121"/>
+    <mergeCell ref="B120:B121"/>
+    <mergeCell ref="A102:A103"/>
+    <mergeCell ref="B102:B103"/>
+    <mergeCell ref="A104:A105"/>
+    <mergeCell ref="B104:B105"/>
+    <mergeCell ref="A106:A107"/>
+    <mergeCell ref="B106:B107"/>
+    <mergeCell ref="A108:A109"/>
+    <mergeCell ref="B108:B109"/>
+    <mergeCell ref="A110:A111"/>
+    <mergeCell ref="B110:B111"/>
+    <mergeCell ref="A92:A93"/>
+    <mergeCell ref="B92:B93"/>
+    <mergeCell ref="A94:A95"/>
+    <mergeCell ref="B94:B95"/>
+    <mergeCell ref="A96:A97"/>
+    <mergeCell ref="B96:B97"/>
+    <mergeCell ref="A98:A99"/>
+    <mergeCell ref="B98:B99"/>
+    <mergeCell ref="A100:A101"/>
+    <mergeCell ref="B100:B101"/>
+    <mergeCell ref="A82:A83"/>
+    <mergeCell ref="B82:B83"/>
+    <mergeCell ref="A84:A85"/>
+    <mergeCell ref="B84:B85"/>
+    <mergeCell ref="A86:A87"/>
+    <mergeCell ref="B86:B87"/>
+    <mergeCell ref="A88:A89"/>
+    <mergeCell ref="B88:B89"/>
+    <mergeCell ref="A90:A91"/>
+    <mergeCell ref="B90:B91"/>
+    <mergeCell ref="A72:A73"/>
+    <mergeCell ref="B72:B73"/>
+    <mergeCell ref="A74:A75"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="A76:A77"/>
+    <mergeCell ref="B76:B77"/>
+    <mergeCell ref="A78:A79"/>
+    <mergeCell ref="B78:B79"/>
+    <mergeCell ref="A80:A81"/>
+    <mergeCell ref="B80:B81"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="A64:A65"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="A66:A67"/>
+    <mergeCell ref="B66:B67"/>
+    <mergeCell ref="A68:A69"/>
+    <mergeCell ref="B68:B69"/>
+    <mergeCell ref="A70:A71"/>
+    <mergeCell ref="B70:B71"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="A4:A5"/>
@@ -7779,196 +7871,6 @@
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B10:B11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="A64:A65"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="A66:A67"/>
-    <mergeCell ref="B66:B67"/>
-    <mergeCell ref="A68:A69"/>
-    <mergeCell ref="B68:B69"/>
-    <mergeCell ref="A70:A71"/>
-    <mergeCell ref="B70:B71"/>
-    <mergeCell ref="A72:A73"/>
-    <mergeCell ref="B72:B73"/>
-    <mergeCell ref="A74:A75"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="A76:A77"/>
-    <mergeCell ref="B76:B77"/>
-    <mergeCell ref="A78:A79"/>
-    <mergeCell ref="B78:B79"/>
-    <mergeCell ref="A80:A81"/>
-    <mergeCell ref="B80:B81"/>
-    <mergeCell ref="A82:A83"/>
-    <mergeCell ref="B82:B83"/>
-    <mergeCell ref="A84:A85"/>
-    <mergeCell ref="B84:B85"/>
-    <mergeCell ref="A86:A87"/>
-    <mergeCell ref="B86:B87"/>
-    <mergeCell ref="A88:A89"/>
-    <mergeCell ref="B88:B89"/>
-    <mergeCell ref="A90:A91"/>
-    <mergeCell ref="B90:B91"/>
-    <mergeCell ref="A92:A93"/>
-    <mergeCell ref="B92:B93"/>
-    <mergeCell ref="A94:A95"/>
-    <mergeCell ref="B94:B95"/>
-    <mergeCell ref="A96:A97"/>
-    <mergeCell ref="B96:B97"/>
-    <mergeCell ref="A98:A99"/>
-    <mergeCell ref="B98:B99"/>
-    <mergeCell ref="A100:A101"/>
-    <mergeCell ref="B100:B101"/>
-    <mergeCell ref="A102:A103"/>
-    <mergeCell ref="B102:B103"/>
-    <mergeCell ref="A104:A105"/>
-    <mergeCell ref="B104:B105"/>
-    <mergeCell ref="A106:A107"/>
-    <mergeCell ref="B106:B107"/>
-    <mergeCell ref="A108:A109"/>
-    <mergeCell ref="B108:B109"/>
-    <mergeCell ref="A110:A111"/>
-    <mergeCell ref="B110:B111"/>
-    <mergeCell ref="A112:A113"/>
-    <mergeCell ref="B112:B113"/>
-    <mergeCell ref="A114:A115"/>
-    <mergeCell ref="B114:B115"/>
-    <mergeCell ref="A116:A117"/>
-    <mergeCell ref="B116:B117"/>
-    <mergeCell ref="A118:A119"/>
-    <mergeCell ref="B118:B119"/>
-    <mergeCell ref="A120:A121"/>
-    <mergeCell ref="B120:B121"/>
-    <mergeCell ref="A122:A123"/>
-    <mergeCell ref="B122:B123"/>
-    <mergeCell ref="A124:A125"/>
-    <mergeCell ref="B124:B125"/>
-    <mergeCell ref="A126:A127"/>
-    <mergeCell ref="B126:B127"/>
-    <mergeCell ref="A128:A129"/>
-    <mergeCell ref="B128:B129"/>
-    <mergeCell ref="A130:A131"/>
-    <mergeCell ref="B130:B131"/>
-    <mergeCell ref="A132:A133"/>
-    <mergeCell ref="B132:B133"/>
-    <mergeCell ref="A134:A135"/>
-    <mergeCell ref="B134:B135"/>
-    <mergeCell ref="A136:A137"/>
-    <mergeCell ref="B136:B137"/>
-    <mergeCell ref="A138:A139"/>
-    <mergeCell ref="B138:B139"/>
-    <mergeCell ref="A140:A141"/>
-    <mergeCell ref="B140:B141"/>
-    <mergeCell ref="A142:A143"/>
-    <mergeCell ref="B142:B143"/>
-    <mergeCell ref="A144:A145"/>
-    <mergeCell ref="B144:B145"/>
-    <mergeCell ref="A146:A147"/>
-    <mergeCell ref="B146:B147"/>
-    <mergeCell ref="A148:A149"/>
-    <mergeCell ref="B148:B149"/>
-    <mergeCell ref="A150:A151"/>
-    <mergeCell ref="B150:B151"/>
-    <mergeCell ref="A152:A153"/>
-    <mergeCell ref="B152:B153"/>
-    <mergeCell ref="A154:A155"/>
-    <mergeCell ref="B154:B155"/>
-    <mergeCell ref="A156:A157"/>
-    <mergeCell ref="B156:B157"/>
-    <mergeCell ref="A158:A159"/>
-    <mergeCell ref="B158:B159"/>
-    <mergeCell ref="A160:A161"/>
-    <mergeCell ref="B160:B161"/>
-    <mergeCell ref="A162:A163"/>
-    <mergeCell ref="B162:B163"/>
-    <mergeCell ref="A164:A165"/>
-    <mergeCell ref="B164:B165"/>
-    <mergeCell ref="A166:A167"/>
-    <mergeCell ref="B166:B167"/>
-    <mergeCell ref="A168:A169"/>
-    <mergeCell ref="B168:B169"/>
-    <mergeCell ref="A170:A171"/>
-    <mergeCell ref="B170:B171"/>
-    <mergeCell ref="A172:A173"/>
-    <mergeCell ref="B172:B173"/>
-    <mergeCell ref="A174:A175"/>
-    <mergeCell ref="B174:B175"/>
-    <mergeCell ref="A176:A177"/>
-    <mergeCell ref="B176:B177"/>
-    <mergeCell ref="A178:A179"/>
-    <mergeCell ref="B178:B179"/>
-    <mergeCell ref="A180:A181"/>
-    <mergeCell ref="B180:B181"/>
-    <mergeCell ref="A182:A183"/>
-    <mergeCell ref="B182:B183"/>
-    <mergeCell ref="A184:A185"/>
-    <mergeCell ref="B184:B185"/>
-    <mergeCell ref="A186:A187"/>
-    <mergeCell ref="B186:B187"/>
-    <mergeCell ref="A188:A189"/>
-    <mergeCell ref="B188:B189"/>
-    <mergeCell ref="A190:A191"/>
-    <mergeCell ref="B190:B191"/>
-    <mergeCell ref="A192:A193"/>
-    <mergeCell ref="B192:B193"/>
-    <mergeCell ref="A194:A195"/>
-    <mergeCell ref="B194:B195"/>
-    <mergeCell ref="A196:A197"/>
-    <mergeCell ref="B196:B197"/>
-    <mergeCell ref="A198:A199"/>
-    <mergeCell ref="B198:B199"/>
-    <mergeCell ref="A200:A201"/>
-    <mergeCell ref="B200:B201"/>
   </mergeCells>
   <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="containsText" priority="1" operator="containsText" text="[UNMATCHED]">

</xml_diff>